<commit_message>
Removendo o validação de valor do recibo no banco de dados
</commit_message>
<xml_diff>
--- a/dadosRecibo.xlsx
+++ b/dadosRecibo.xlsx
@@ -1,32 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto Botcity\leituraPDF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B2C9E5-1675-4990-94B6-AF689E4AD83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Profissional</t>
+  </si>
+  <si>
+    <t>Descrição do Serviço</t>
+  </si>
+  <si>
+    <t>Forma de Pagamento</t>
+  </si>
+  <si>
+    <t>Data do Pagamento</t>
+  </si>
+  <si>
+    <t>SubTotal</t>
+  </si>
+  <si>
+    <t>Basic System</t>
+  </si>
+  <si>
+    <t>Desenvolvedor: Maria Lima</t>
+  </si>
+  <si>
+    <t>Raspagem de Dados, Leitura PDF</t>
+  </si>
+  <si>
+    <t>Pagamento na Entrega</t>
+  </si>
+  <si>
+    <t>30/08/2023</t>
+  </si>
+  <si>
+    <t>470,00</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -42,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,33 +89,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -114,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -148,7 +197,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -183,10 +231,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -359,15 +406,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>